<commit_message>
Analyse af damp proces
</commit_message>
<xml_diff>
--- a/statisk-analyse.xlsx
+++ b/statisk-analyse.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Proces M7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnu\Desktop\MSK M7\SharedFolder studie5000\OB2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813F43EE-2D8F-48CF-98B4-B3391A42CCBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDB412A-C393-4F93-8D90-0EFB84065C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3EF89485-D765-448B-8C81-FCD90405C393}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{3EF89485-D765-448B-8C81-FCD90405C393}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t xml:space="preserve">Statisk analyse </t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t xml:space="preserve">15 sek </t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>19 sek</t>
   </si>
 </sst>
 </file>
@@ -206,9 +212,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -251,7 +256,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="da-DK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -313,15 +318,25 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="da-DK"/>
+          <a:endParaRPr lang="en-DK"/>
         </a:p>
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.7171065999407275E-2"/>
+          <c:y val="9.5527019579027331E-2"/>
+          <c:w val="0.80580690115898157"/>
+          <c:h val="0.84880129875182142"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -388,7 +403,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="da-DK"/>
+                <a:endParaRPr lang="en-DK"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -503,7 +518,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-82FD-46EF-82A3-3A0D553F9613}"/>
@@ -575,7 +590,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="da-DK"/>
+                <a:endParaRPr lang="en-DK"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -690,7 +705,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-82FD-46EF-82A3-3A0D553F9613}"/>
@@ -762,7 +777,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="da-DK"/>
+                <a:endParaRPr lang="en-DK"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -877,10 +892,197 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-82FD-46EF-82A3-3A0D553F9613}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ark1'!$C$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Damp proces </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-DK"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ark1'!$E$4:$O$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ark1'!$E$8:$O$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8249-471B-866D-77FCA0D2946A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -951,7 +1153,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="da-DK"/>
+            <a:endParaRPr lang="en-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="460598816"/>
@@ -1013,7 +1215,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="da-DK"/>
+            <a:endParaRPr lang="en-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="460595208"/>
@@ -1055,7 +1257,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="da-DK"/>
+          <a:endParaRPr lang="en-DK"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1092,7 +1294,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="da-DK"/>
+      <a:endParaRPr lang="en-DK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1663,16 +1865,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1199029</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>347382</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:rowOff>184149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>493059</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>78441</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>18676</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1701,7 +1903,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1997,315 +2199,366 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{347E4FF2-77BA-454E-9F98-7E4D032D447D}">
-  <dimension ref="B3:O51"/>
+  <dimension ref="B3:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8" t="s">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="9"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="8"/>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>0</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>10</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>20</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>30</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>40</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <v>50</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <v>60</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <v>70</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="3">
         <v>80</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="3">
         <v>90</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="3">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="4" t="s">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>15</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>0</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>7.2</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>32.4</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>57.6</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>82.8</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <v>100</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="4">
         <v>100</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="4">
         <v>100</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="4">
         <v>100</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="4">
         <v>100</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C6" s="4" t="s">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>10</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>0</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>7.8</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>27.6</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>47.4</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>67.2</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="4">
         <v>87</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="4">
         <v>100</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="4">
         <v>100</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="4">
         <v>100</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="4">
         <v>100</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C7" s="4" t="s">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>7</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>0</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>2.8</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>15.4</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>28</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <v>40.6</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="4">
         <v>53.2</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="4">
         <v>65.8</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="4">
         <v>78.400000000000006</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="4">
         <v>91</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="4">
         <v>100</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="4" t="s">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
+      <c r="D8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="4">
+        <v>15</v>
+      </c>
+      <c r="F8" s="4">
+        <v>13.5</v>
+      </c>
+      <c r="G8" s="4">
+        <v>12</v>
+      </c>
+      <c r="H8" s="4">
+        <v>10.5</v>
+      </c>
+      <c r="I8" s="4">
+        <v>9</v>
+      </c>
+      <c r="J8" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="K8" s="4">
+        <v>6</v>
+      </c>
+      <c r="L8" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="M8" s="4">
+        <v>3</v>
+      </c>
+      <c r="N8" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="11"/>
-      <c r="C41" s="11" t="s">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B41" s="10"/>
+      <c r="C41" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="11" t="s">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B42" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="11">
-        <v>12.6</v>
-      </c>
-      <c r="D42" s="11">
+      <c r="C42" s="10">
+        <f>I5-H5</f>
+        <v>25.199999999999996</v>
+      </c>
+      <c r="D42" s="10">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="11" t="s">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B43" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="11">
-        <v>19.8</v>
-      </c>
-      <c r="D43" s="11">
+      <c r="C43" s="10">
+        <f t="shared" ref="C43:C45" si="0">I6-H6</f>
+        <v>19.800000000000004</v>
+      </c>
+      <c r="D43" s="10">
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="11" t="s">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B44" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C44" s="11">
-        <v>25.2</v>
-      </c>
-      <c r="D44" s="11">
+      <c r="C44" s="10">
+        <f t="shared" si="0"/>
+        <v>12.600000000000001</v>
+      </c>
+      <c r="D44" s="10">
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="10"/>
-      <c r="C48" s="10" t="s">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C45" s="10">
+        <f t="shared" si="0"/>
+        <v>-1.5</v>
+      </c>
+      <c r="D45" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B48" s="9"/>
+      <c r="C48" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="D48" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="10" t="s">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B49" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C49" s="4">
         <f>C42/D42</f>
-        <v>1.26</v>
-      </c>
-      <c r="D49" s="5" t="s">
+        <v>2.5199999999999996</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E49" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="10" t="s">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B50" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C50" s="4">
         <f>C43/D43</f>
-        <v>1.98</v>
-      </c>
-      <c r="D50" s="5" t="s">
+        <v>1.9800000000000004</v>
+      </c>
+      <c r="D50" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="E50" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="10" t="s">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B51" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C51" s="4">
         <f>C44/D44</f>
-        <v>2.52</v>
-      </c>
-      <c r="D51" s="5" t="s">
+        <v>1.2600000000000002</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E51" s="5" t="s">
+      <c r="E51" s="4" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B52" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="4">
+        <f>C45/D45</f>
+        <v>-0.15</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>